<commit_message>
Added product report and export component
</commit_message>
<xml_diff>
--- a/lao20180315.xlsx
+++ b/lao20180315.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\LayAwayOnlineETL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" url="C:\Project\LayAwayOnlineETL\"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" r:id="rId1"/>
-    <sheet name="Warranty" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" r:id="rId1" name="Items"/>
+    <sheet sheetId="2" r:id="rId2" name="Warranty"/>
+    <sheet r:id="rId6" name="Excel_Destination" sheetId="3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="Excel_Destination">'Excel_Destination'!$A$1:$N$1</definedName>
+  </definedNames>
+  <calcPr calcId="144525" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66792,4 +66792,35 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>